<commit_message>
got new letters for alpha
</commit_message>
<xml_diff>
--- a/Compiled Yields.xlsx
+++ b/Compiled Yields.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kentp\Documents\GitHub\Rhizosphere-sequencing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F5908C8-3C77-4C9F-BB4D-D4602E345CDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42A28746-FBB0-4236-A268-1472E8257F1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="17115" windowHeight="10876" xr2:uid="{DC883E9F-58DC-A14C-A68E-C7566C858015}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="23">
   <si>
     <t>Plot</t>
   </si>
@@ -71,13 +71,7 @@
     <t>Sample_ID</t>
   </si>
   <si>
-    <t>CC1</t>
-  </si>
-  <si>
     <t>HF1</t>
-  </si>
-  <si>
-    <t>CC2</t>
   </si>
   <si>
     <t>HG1</t>
@@ -93,6 +87,24 @@
   </si>
   <si>
     <t>Stover</t>
+  </si>
+  <si>
+    <t>Treatment</t>
+  </si>
+  <si>
+    <t>CT1</t>
+  </si>
+  <si>
+    <t>CT2</t>
+  </si>
+  <si>
+    <t>Conventional</t>
+  </si>
+  <si>
+    <t>Hemp Fiber</t>
+  </si>
+  <si>
+    <t>Hemp Grain</t>
   </si>
 </sst>
 </file>
@@ -506,22 +518,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDB5AC9C-1D94-7546-810B-A6D94125F5C2}">
-  <dimension ref="A1:J91"/>
+  <dimension ref="A1:K91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K78" sqref="A1:XFD1048576"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="10.8125" style="1"/>
-    <col min="2" max="2" width="14.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.8125" style="1"/>
-    <col min="6" max="8" width="11.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" style="1"/>
+    <col min="3" max="3" width="14.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.8125" style="1"/>
+    <col min="7" max="9" width="11.5" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -529,2966 +542,3239 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.5">
+        <v>15</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A2" s="2">
         <v>106</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>2021</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2" s="2">
         <v>106</v>
       </c>
-      <c r="F2" s="4">
+      <c r="G2" s="4">
         <v>10382.333333333334</v>
       </c>
-      <c r="G2" s="4">
+      <c r="H2" s="4">
         <v>9720</v>
       </c>
-      <c r="H2" s="5">
+      <c r="I2" s="5">
         <v>20102.333333333336</v>
       </c>
-      <c r="I2" s="4">
+      <c r="J2" s="4">
         <v>9720</v>
       </c>
-      <c r="J2" s="6">
-        <f>H2-I2</f>
+      <c r="K2" s="6">
+        <f>I2-J2</f>
         <v>10382.333333333336</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A3" s="2">
         <v>202</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>2021</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3" s="2">
         <v>202</v>
       </c>
-      <c r="F3" s="4">
+      <c r="G3" s="4">
         <v>10109.189189189185</v>
       </c>
-      <c r="G3" s="4">
+      <c r="H3" s="4">
         <v>9900</v>
       </c>
-      <c r="H3" s="5">
+      <c r="I3" s="5">
         <v>20009.189189189186</v>
       </c>
-      <c r="I3" s="4">
+      <c r="J3" s="4">
         <v>9900</v>
       </c>
-      <c r="J3" s="6">
-        <f t="shared" ref="J3:J66" si="0">H3-I3</f>
+      <c r="K3" s="6">
+        <f t="shared" ref="K3:K66" si="0">I3-J3</f>
         <v>10109.189189189186</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A4" s="2">
         <v>301</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="1">
         <v>2021</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F4" s="2">
         <v>301</v>
       </c>
-      <c r="F4" s="4">
+      <c r="G4" s="4">
         <v>9326.0674157303365</v>
       </c>
-      <c r="G4" s="4">
+      <c r="H4" s="4">
         <v>9560</v>
       </c>
-      <c r="H4" s="5">
+      <c r="I4" s="5">
         <v>18886.067415730337</v>
       </c>
-      <c r="I4" s="4">
+      <c r="J4" s="4">
         <v>9560</v>
       </c>
-      <c r="J4" s="6">
+      <c r="K4" s="6">
         <f t="shared" si="0"/>
         <v>9326.0674157303365</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A5" s="2">
         <v>405</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <v>2021</v>
       </c>
-      <c r="E5" s="2">
+      <c r="F5" s="2">
         <v>405</v>
       </c>
-      <c r="F5" s="4">
+      <c r="G5" s="4">
         <v>7503.1906614785985</v>
       </c>
-      <c r="G5" s="4">
+      <c r="H5" s="4">
         <v>11300.000000000002</v>
       </c>
-      <c r="H5" s="5">
+      <c r="I5" s="5">
         <v>18803.190661478598</v>
       </c>
-      <c r="I5" s="4">
+      <c r="J5" s="4">
         <v>11300.000000000002</v>
       </c>
-      <c r="J5" s="6">
+      <c r="K5" s="6">
         <f t="shared" si="0"/>
         <v>7503.1906614785967</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A6" s="2">
         <v>504</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6" s="1">
         <v>2021</v>
       </c>
-      <c r="E6" s="2">
+      <c r="F6" s="2">
         <v>504</v>
       </c>
-      <c r="F6" s="4">
+      <c r="G6" s="4">
         <v>8176.9811320754716</v>
       </c>
-      <c r="G6" s="4">
+      <c r="H6" s="4">
         <v>8800.0000000000018</v>
       </c>
-      <c r="H6" s="5">
+      <c r="I6" s="5">
         <v>16976.981132075474</v>
       </c>
-      <c r="I6" s="4">
+      <c r="J6" s="4">
         <v>8800.0000000000018</v>
       </c>
-      <c r="J6" s="6">
+      <c r="K6" s="6">
         <f t="shared" si="0"/>
         <v>8176.9811320754725</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A7" s="3">
         <v>104</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="1">
+      <c r="E7" s="1">
         <v>2021</v>
       </c>
-      <c r="E7" s="3">
+      <c r="F7" s="3">
         <v>104</v>
       </c>
-      <c r="F7" s="4">
+      <c r="G7" s="4">
         <v>4500</v>
       </c>
-      <c r="G7" s="4"/>
-      <c r="H7" s="5">
+      <c r="H7" s="4"/>
+      <c r="I7" s="5">
         <v>4500</v>
       </c>
-      <c r="I7" s="4">
+      <c r="J7" s="4">
         <v>4500</v>
       </c>
-      <c r="J7" s="6">
+      <c r="K7" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A8" s="3">
         <v>206</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="1">
+      <c r="E8" s="1">
         <v>2021</v>
       </c>
-      <c r="E8" s="3">
+      <c r="F8" s="3">
         <v>206</v>
       </c>
-      <c r="F8" s="4">
+      <c r="G8" s="4">
         <v>8480</v>
       </c>
-      <c r="G8" s="4"/>
-      <c r="H8" s="5">
+      <c r="H8" s="4"/>
+      <c r="I8" s="5">
         <v>8480</v>
       </c>
-      <c r="I8" s="4">
+      <c r="J8" s="4">
         <v>8480</v>
       </c>
-      <c r="J8" s="6">
+      <c r="K8" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A9" s="3">
         <v>306</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="1">
+      <c r="E9" s="1">
         <v>2021</v>
       </c>
-      <c r="E9" s="3">
+      <c r="F9" s="3">
         <v>306</v>
       </c>
-      <c r="F9" s="4">
+      <c r="G9" s="4">
         <v>1160.0000000000002</v>
       </c>
-      <c r="G9" s="4"/>
-      <c r="H9" s="5">
+      <c r="H9" s="4"/>
+      <c r="I9" s="5">
         <v>1160.0000000000002</v>
       </c>
-      <c r="I9" s="4">
+      <c r="J9" s="4">
         <v>1160.0000000000002</v>
       </c>
-      <c r="J9" s="6">
+      <c r="K9" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A10" s="3">
         <v>403</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="1">
+      <c r="E10" s="1">
         <v>2021</v>
       </c>
-      <c r="E10" s="3">
+      <c r="F10" s="3">
         <v>403</v>
       </c>
-      <c r="F10" s="4">
+      <c r="G10" s="4">
         <v>9840</v>
       </c>
-      <c r="G10" s="4"/>
-      <c r="H10" s="5">
+      <c r="H10" s="4"/>
+      <c r="I10" s="5">
         <v>9840</v>
       </c>
-      <c r="I10" s="4">
+      <c r="J10" s="4">
         <v>9840</v>
       </c>
-      <c r="J10" s="6">
+      <c r="K10" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A11" s="3">
         <v>501</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="1">
+      <c r="E11" s="1">
         <v>2021</v>
       </c>
-      <c r="E11" s="3">
+      <c r="F11" s="3">
         <v>501</v>
       </c>
-      <c r="F11" s="4">
+      <c r="G11" s="4">
         <v>9840</v>
       </c>
-      <c r="G11" s="4"/>
-      <c r="H11" s="5">
+      <c r="H11" s="4"/>
+      <c r="I11" s="5">
         <v>9840</v>
       </c>
-      <c r="I11" s="4">
+      <c r="J11" s="4">
         <v>9840</v>
       </c>
-      <c r="J11" s="6">
+      <c r="K11" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A12" s="2">
         <v>103</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="1">
+      <c r="E12" s="1">
         <v>2021</v>
       </c>
-      <c r="E12" s="2">
+      <c r="F12" s="2">
         <v>103</v>
       </c>
-      <c r="F12" s="4">
+      <c r="G12" s="4">
         <v>3551.9999999999995</v>
       </c>
-      <c r="G12" s="4">
+      <c r="H12" s="4">
         <v>4428</v>
       </c>
-      <c r="H12" s="5">
+      <c r="I12" s="5">
         <v>7980</v>
       </c>
-      <c r="I12" s="4">
+      <c r="J12" s="4">
         <v>4428</v>
       </c>
-      <c r="J12" s="6">
+      <c r="K12" s="6">
         <f t="shared" si="0"/>
         <v>3552</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A13" s="2">
         <v>204</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="1">
+      <c r="E13" s="1">
         <v>2021</v>
       </c>
-      <c r="E13" s="2">
+      <c r="F13" s="2">
         <v>204</v>
       </c>
-      <c r="F13" s="4">
+      <c r="G13" s="4">
         <v>4731.9999999999982</v>
       </c>
-      <c r="G13" s="4">
+      <c r="H13" s="4">
         <v>5008</v>
       </c>
-      <c r="H13" s="5">
+      <c r="I13" s="5">
         <v>9739.9999999999982</v>
       </c>
-      <c r="I13" s="4">
+      <c r="J13" s="4">
         <v>5008</v>
       </c>
-      <c r="J13" s="6">
+      <c r="K13" s="6">
         <f t="shared" si="0"/>
         <v>4731.9999999999982</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A14" s="2">
         <v>305</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="1">
+      <c r="E14" s="1">
         <v>2021</v>
       </c>
-      <c r="E14" s="2">
+      <c r="F14" s="2">
         <v>305</v>
       </c>
-      <c r="F14" s="4">
+      <c r="G14" s="4">
         <v>5551.9999999999991</v>
       </c>
-      <c r="G14" s="4">
+      <c r="H14" s="4">
         <v>5488</v>
       </c>
-      <c r="H14" s="5">
+      <c r="I14" s="5">
         <v>11040</v>
       </c>
-      <c r="I14" s="4">
+      <c r="J14" s="4">
         <v>5488</v>
       </c>
-      <c r="J14" s="6">
+      <c r="K14" s="6">
         <f t="shared" si="0"/>
         <v>5552</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A15" s="2">
         <v>401</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="1">
+      <c r="E15" s="1">
         <v>2021</v>
       </c>
-      <c r="E15" s="2">
+      <c r="F15" s="2">
         <v>401</v>
       </c>
-      <c r="F15" s="4">
+      <c r="G15" s="4">
         <v>4872</v>
       </c>
-      <c r="G15" s="4">
+      <c r="H15" s="4">
         <v>5568</v>
       </c>
-      <c r="H15" s="5">
+      <c r="I15" s="5">
         <v>10440</v>
       </c>
-      <c r="I15" s="4">
+      <c r="J15" s="4">
         <v>5568</v>
       </c>
-      <c r="J15" s="6">
+      <c r="K15" s="6">
         <f t="shared" si="0"/>
         <v>4872</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A16" s="2">
         <v>502</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="1">
+      <c r="E16" s="1">
         <v>2021</v>
       </c>
-      <c r="E16" s="2">
+      <c r="F16" s="2">
         <v>502</v>
       </c>
-      <c r="F16" s="4">
+      <c r="G16" s="4">
         <v>3631.9999999999995</v>
       </c>
-      <c r="G16" s="4">
+      <c r="H16" s="4">
         <v>4107.9999999999991</v>
       </c>
-      <c r="H16" s="5">
+      <c r="I16" s="5">
         <v>7739.9999999999982</v>
       </c>
-      <c r="I16" s="4">
+      <c r="J16" s="4">
         <v>4107.9999999999991</v>
       </c>
-      <c r="J16" s="6">
+      <c r="K16" s="6">
         <f t="shared" si="0"/>
         <v>3631.9999999999991</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A17" s="1">
         <v>105</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>14</v>
+      <c r="B17" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="1">
+      <c r="E17" s="1">
         <v>2021</v>
       </c>
-      <c r="E17" s="1">
+      <c r="F17" s="1">
         <v>105</v>
       </c>
-      <c r="F17" s="4">
+      <c r="G17" s="4">
         <v>5858</v>
       </c>
-      <c r="G17" s="4">
+      <c r="H17" s="4">
         <v>982</v>
       </c>
-      <c r="H17" s="5">
+      <c r="I17" s="5">
         <v>6840</v>
       </c>
-      <c r="I17" s="4">
+      <c r="J17" s="4">
         <v>982</v>
       </c>
-      <c r="J17" s="6">
+      <c r="K17" s="6">
         <f t="shared" si="0"/>
         <v>5858</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A18" s="1">
         <v>203</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>14</v>
+      <c r="B18" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="1">
+      <c r="E18" s="1">
         <v>2021</v>
       </c>
-      <c r="E18" s="1">
+      <c r="F18" s="1">
         <v>203</v>
       </c>
-      <c r="F18" s="4">
+      <c r="G18" s="4">
         <v>5943.9999999999991</v>
       </c>
-      <c r="G18" s="4">
+      <c r="H18" s="4">
         <v>1116</v>
       </c>
-      <c r="H18" s="5">
+      <c r="I18" s="5">
         <v>7059.9999999999991</v>
       </c>
-      <c r="I18" s="4">
+      <c r="J18" s="4">
         <v>1116</v>
       </c>
-      <c r="J18" s="6">
+      <c r="K18" s="6">
         <f t="shared" si="0"/>
         <v>5943.9999999999991</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A19" s="1">
         <v>302</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>14</v>
+      <c r="B19" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D19" s="1">
+      <c r="E19" s="1">
         <v>2021</v>
       </c>
-      <c r="E19" s="1">
+      <c r="F19" s="1">
         <v>302</v>
       </c>
-      <c r="F19" s="4">
+      <c r="G19" s="4">
         <v>4053.9999999999991</v>
       </c>
-      <c r="G19" s="4">
+      <c r="H19" s="4">
         <v>626</v>
       </c>
-      <c r="H19" s="5">
+      <c r="I19" s="5">
         <v>4679.9999999999991</v>
       </c>
-      <c r="I19" s="4">
+      <c r="J19" s="4">
         <v>626</v>
       </c>
-      <c r="J19" s="6">
+      <c r="K19" s="6">
         <f t="shared" si="0"/>
         <v>4053.9999999999991</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A20" s="1">
         <v>406</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>14</v>
+      <c r="B20" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="1">
+      <c r="E20" s="1">
         <v>2021</v>
       </c>
-      <c r="E20" s="1">
+      <c r="F20" s="1">
         <v>406</v>
       </c>
-      <c r="F20" s="4">
+      <c r="G20" s="4">
         <v>6092.0000000000009</v>
       </c>
-      <c r="G20" s="4">
+      <c r="H20" s="4">
         <v>888</v>
       </c>
-      <c r="H20" s="5">
+      <c r="I20" s="5">
         <v>6980.0000000000009</v>
       </c>
-      <c r="I20" s="4">
+      <c r="J20" s="4">
         <v>888</v>
       </c>
-      <c r="J20" s="6">
+      <c r="K20" s="6">
         <f t="shared" si="0"/>
         <v>6092.0000000000009</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A21" s="1">
         <v>503</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>14</v>
+      <c r="B21" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D21" s="1">
+      <c r="E21" s="1">
         <v>2021</v>
       </c>
-      <c r="E21" s="1">
+      <c r="F21" s="1">
         <v>503</v>
       </c>
-      <c r="F21" s="4">
+      <c r="G21" s="4">
         <v>5014.0000000000009</v>
       </c>
-      <c r="G21" s="4">
+      <c r="H21" s="4">
         <v>965.99999999999989</v>
       </c>
-      <c r="H21" s="5">
+      <c r="I21" s="5">
         <v>5980.0000000000009</v>
       </c>
-      <c r="I21" s="4">
+      <c r="J21" s="4">
         <v>965.99999999999989</v>
       </c>
-      <c r="J21" s="6">
+      <c r="K21" s="6">
         <f t="shared" si="0"/>
         <v>5014.0000000000009</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A22" s="2">
         <v>101</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>15</v>
+      <c r="B22" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="C22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="1">
+      <c r="E22" s="1">
         <v>2021</v>
       </c>
-      <c r="E22" s="2">
+      <c r="F22" s="2">
         <v>101</v>
       </c>
-      <c r="F22" s="4">
+      <c r="G22" s="4">
         <v>3471.9999999999995</v>
       </c>
-      <c r="G22" s="4">
+      <c r="H22" s="4">
         <v>4268</v>
       </c>
-      <c r="H22" s="5">
+      <c r="I22" s="5">
         <v>7740</v>
       </c>
-      <c r="I22" s="4">
+      <c r="J22" s="4">
         <v>4268</v>
       </c>
-      <c r="J22" s="6">
+      <c r="K22" s="6">
         <f t="shared" si="0"/>
         <v>3472</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A23" s="2">
         <v>205</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>15</v>
+      <c r="B23" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="C23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="1">
+      <c r="E23" s="1">
         <v>2021</v>
       </c>
-      <c r="E23" s="2">
+      <c r="F23" s="2">
         <v>205</v>
       </c>
-      <c r="F23" s="4">
+      <c r="G23" s="4">
         <v>4571.9999999999991</v>
       </c>
-      <c r="G23" s="4">
+      <c r="H23" s="4">
         <v>4568</v>
       </c>
-      <c r="H23" s="5">
+      <c r="I23" s="5">
         <v>9140</v>
       </c>
-      <c r="I23" s="4">
+      <c r="J23" s="4">
         <v>4568</v>
       </c>
-      <c r="J23" s="6">
+      <c r="K23" s="6">
         <f t="shared" si="0"/>
         <v>4572</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A24" s="2">
         <v>303</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>15</v>
+      <c r="B24" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="C24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D24" s="1">
+      <c r="E24" s="1">
         <v>2021</v>
       </c>
-      <c r="E24" s="2">
+      <c r="F24" s="2">
         <v>303</v>
       </c>
-      <c r="F24" s="4">
+      <c r="G24" s="4">
         <v>6612</v>
       </c>
-      <c r="G24" s="4">
+      <c r="H24" s="4">
         <v>4728</v>
       </c>
-      <c r="H24" s="5">
+      <c r="I24" s="5">
         <v>11340</v>
       </c>
-      <c r="I24" s="4">
+      <c r="J24" s="4">
         <v>4728</v>
       </c>
-      <c r="J24" s="6">
+      <c r="K24" s="6">
         <f t="shared" si="0"/>
         <v>6612</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A25" s="2">
         <v>404</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>15</v>
+      <c r="B25" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="C25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D25" s="1">
+      <c r="E25" s="1">
         <v>2021</v>
       </c>
-      <c r="E25" s="2">
+      <c r="F25" s="2">
         <v>404</v>
       </c>
-      <c r="F25" s="4">
+      <c r="G25" s="4">
         <v>3671.9999999999986</v>
       </c>
-      <c r="G25" s="4">
+      <c r="H25" s="4">
         <v>5368.0000000000009</v>
       </c>
-      <c r="H25" s="5">
+      <c r="I25" s="5">
         <v>9040</v>
       </c>
-      <c r="I25" s="4">
+      <c r="J25" s="4">
         <v>5368.0000000000009</v>
       </c>
-      <c r="J25" s="6">
+      <c r="K25" s="6">
         <f t="shared" si="0"/>
         <v>3671.9999999999991</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A26" s="2">
         <v>506</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>15</v>
+      <c r="B26" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="C26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D26" s="1">
+      <c r="E26" s="1">
         <v>2021</v>
       </c>
-      <c r="E26" s="2">
+      <c r="F26" s="2">
         <v>506</v>
       </c>
-      <c r="F26" s="4">
+      <c r="G26" s="4">
         <v>5151.9999999999991</v>
       </c>
-      <c r="G26" s="4">
+      <c r="H26" s="4">
         <v>4428</v>
       </c>
-      <c r="H26" s="5">
+      <c r="I26" s="5">
         <v>9580</v>
       </c>
-      <c r="I26" s="4">
+      <c r="J26" s="4">
         <v>4428</v>
       </c>
-      <c r="J26" s="6">
+      <c r="K26" s="6">
         <f t="shared" si="0"/>
         <v>5152</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A27" s="2">
         <v>102</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C27" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D27" s="1">
+      <c r="E27" s="1">
         <v>2021</v>
       </c>
-      <c r="E27" s="2">
+      <c r="F27" s="2">
         <v>102</v>
       </c>
-      <c r="F27" s="4">
+      <c r="G27" s="4">
         <v>7111.9999999999982</v>
       </c>
-      <c r="G27" s="4">
+      <c r="H27" s="4">
         <v>9340</v>
       </c>
-      <c r="H27" s="5">
+      <c r="I27" s="5">
         <v>16452</v>
       </c>
-      <c r="I27" s="4">
+      <c r="J27" s="4">
         <v>9340</v>
       </c>
-      <c r="J27" s="6">
+      <c r="K27" s="6">
         <f t="shared" si="0"/>
         <v>7112</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A28" s="2">
         <v>201</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C28" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D28" s="1">
+      <c r="E28" s="1">
         <v>2021</v>
       </c>
-      <c r="E28" s="2">
+      <c r="F28" s="2">
         <v>201</v>
       </c>
-      <c r="F28" s="4">
+      <c r="G28" s="4">
         <v>9528.2926829268272</v>
       </c>
-      <c r="G28" s="4">
+      <c r="H28" s="4">
         <v>9560</v>
       </c>
-      <c r="H28" s="5">
+      <c r="I28" s="5">
         <v>19088.292682926825</v>
       </c>
-      <c r="I28" s="4">
+      <c r="J28" s="4">
         <v>9560</v>
       </c>
-      <c r="J28" s="6">
+      <c r="K28" s="6">
         <f t="shared" si="0"/>
         <v>9528.2926829268254</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A29" s="2">
         <v>304</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D29" s="1">
+      <c r="E29" s="1">
         <v>2021</v>
       </c>
-      <c r="E29" s="2">
+      <c r="F29" s="2">
         <v>304</v>
       </c>
-      <c r="F29" s="4">
+      <c r="G29" s="4">
         <v>9214.5991561181399</v>
       </c>
-      <c r="G29" s="4">
+      <c r="H29" s="4">
         <v>10180</v>
       </c>
-      <c r="H29" s="5">
+      <c r="I29" s="5">
         <v>19394.59915611814</v>
       </c>
-      <c r="I29" s="4">
+      <c r="J29" s="4">
         <v>10180</v>
       </c>
-      <c r="J29" s="6">
+      <c r="K29" s="6">
         <f t="shared" si="0"/>
         <v>9214.5991561181399</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A30" s="2">
         <v>402</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C30" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D30" s="1">
+      <c r="E30" s="1">
         <v>2021</v>
       </c>
-      <c r="E30" s="2">
+      <c r="F30" s="2">
         <v>402</v>
       </c>
-      <c r="F30" s="4">
+      <c r="G30" s="4">
         <v>10998.461538461537</v>
       </c>
-      <c r="G30" s="4">
+      <c r="H30" s="4">
         <v>11460.000000000002</v>
       </c>
-      <c r="H30" s="5">
+      <c r="I30" s="5">
         <v>22458.461538461539</v>
       </c>
-      <c r="I30" s="4">
+      <c r="J30" s="4">
         <v>11460.000000000002</v>
       </c>
-      <c r="J30" s="6">
+      <c r="K30" s="6">
         <f t="shared" si="0"/>
         <v>10998.461538461537</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A31" s="2">
         <v>505</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C31" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D31" s="1">
+      <c r="E31" s="1">
         <v>2021</v>
       </c>
-      <c r="E31" s="2">
+      <c r="F31" s="2">
         <v>505</v>
       </c>
-      <c r="F31" s="4">
+      <c r="G31" s="4">
         <v>8272.6315789473683</v>
       </c>
-      <c r="G31" s="4">
+      <c r="H31" s="4">
         <v>8859.9999999999982</v>
       </c>
-      <c r="H31" s="5">
+      <c r="I31" s="5">
         <v>17132.631578947367</v>
       </c>
-      <c r="I31" s="4">
+      <c r="J31" s="4">
         <v>8859.9999999999982</v>
       </c>
-      <c r="J31" s="6">
+      <c r="K31" s="6">
         <f t="shared" si="0"/>
         <v>8272.6315789473683</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A32" s="2">
         <v>106</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C32" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D32" s="1">
+      <c r="E32" s="1">
         <v>2022</v>
       </c>
-      <c r="E32" s="2">
+      <c r="F32" s="2">
         <v>106</v>
       </c>
-      <c r="F32" s="5">
+      <c r="G32" s="5">
         <v>5380</v>
       </c>
-      <c r="G32" s="5">
+      <c r="H32" s="5">
         <v>4520</v>
       </c>
-      <c r="H32" s="5">
+      <c r="I32" s="5">
         <v>9900</v>
       </c>
-      <c r="I32" s="5">
+      <c r="J32" s="5">
         <v>4520</v>
       </c>
-      <c r="J32" s="6">
+      <c r="K32" s="6">
         <f t="shared" si="0"/>
         <v>5380</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A33" s="2">
         <v>202</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C33" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D33" s="1">
+      <c r="E33" s="1">
         <v>2022</v>
       </c>
-      <c r="E33" s="2">
+      <c r="F33" s="2">
         <v>202</v>
       </c>
-      <c r="F33" s="5">
+      <c r="G33" s="5">
         <v>4580</v>
       </c>
-      <c r="G33" s="5">
+      <c r="H33" s="5">
         <v>4500</v>
       </c>
-      <c r="H33" s="5">
+      <c r="I33" s="5">
         <v>9080</v>
       </c>
-      <c r="I33" s="5">
+      <c r="J33" s="5">
         <v>4500</v>
       </c>
-      <c r="J33" s="6">
+      <c r="K33" s="6">
         <f t="shared" si="0"/>
         <v>4580</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A34" s="2">
         <v>301</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C34" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D34" s="1">
+      <c r="E34" s="1">
         <v>2022</v>
       </c>
-      <c r="E34" s="2">
+      <c r="F34" s="2">
         <v>301</v>
       </c>
-      <c r="F34" s="5">
+      <c r="G34" s="5">
         <v>4860</v>
       </c>
-      <c r="G34" s="5">
+      <c r="H34" s="5">
         <v>4120</v>
       </c>
-      <c r="H34" s="5">
+      <c r="I34" s="5">
         <v>8980</v>
       </c>
-      <c r="I34" s="5">
+      <c r="J34" s="5">
         <v>4120</v>
       </c>
-      <c r="J34" s="6">
+      <c r="K34" s="6">
         <f t="shared" si="0"/>
         <v>4860</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A35" s="2">
         <v>405</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C35" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D35" s="1">
+      <c r="E35" s="1">
         <v>2022</v>
       </c>
-      <c r="E35" s="2">
+      <c r="F35" s="2">
         <v>405</v>
       </c>
-      <c r="F35" s="5">
+      <c r="G35" s="5">
         <v>4899.9999999999991</v>
       </c>
-      <c r="G35" s="5">
+      <c r="H35" s="5">
         <v>4300</v>
       </c>
-      <c r="H35" s="5">
+      <c r="I35" s="5">
         <v>9200</v>
       </c>
-      <c r="I35" s="5">
+      <c r="J35" s="5">
         <v>4300</v>
       </c>
-      <c r="J35" s="6">
+      <c r="K35" s="6">
         <f t="shared" si="0"/>
         <v>4900</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A36" s="2">
         <v>504</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C36" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D36" s="1">
+      <c r="E36" s="1">
         <v>2022</v>
       </c>
-      <c r="E36" s="2">
+      <c r="F36" s="2">
         <v>504</v>
       </c>
-      <c r="F36" s="5">
+      <c r="G36" s="5">
         <v>3060</v>
       </c>
-      <c r="G36" s="5">
+      <c r="H36" s="5">
         <v>2320</v>
       </c>
-      <c r="H36" s="5">
+      <c r="I36" s="5">
         <v>5380</v>
       </c>
-      <c r="I36" s="5">
+      <c r="J36" s="5">
         <v>2320</v>
       </c>
-      <c r="J36" s="6">
+      <c r="K36" s="6">
         <f t="shared" si="0"/>
         <v>3060</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A37" s="3">
         <v>104</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C37" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D37" s="1">
+      <c r="E37" s="1">
         <v>2022</v>
       </c>
-      <c r="E37" s="3">
+      <c r="F37" s="3">
         <v>104</v>
       </c>
-      <c r="F37" s="5">
+      <c r="G37" s="5">
         <v>4600</v>
       </c>
-      <c r="G37" s="5">
+      <c r="H37" s="5">
         <v>4240</v>
       </c>
-      <c r="H37" s="5">
+      <c r="I37" s="5">
         <v>8840</v>
       </c>
-      <c r="I37" s="5">
+      <c r="J37" s="5">
         <v>4240</v>
       </c>
-      <c r="J37" s="6">
+      <c r="K37" s="6">
         <f t="shared" si="0"/>
         <v>4600</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A38" s="3">
         <v>206</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C38" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D38" s="1">
+      <c r="E38" s="1">
         <v>2022</v>
       </c>
-      <c r="E38" s="3">
+      <c r="F38" s="3">
         <v>206</v>
       </c>
-      <c r="F38" s="5">
+      <c r="G38" s="5">
         <v>4400.0000000000009</v>
       </c>
-      <c r="G38" s="5">
+      <c r="H38" s="5">
         <v>3399.9999999999995</v>
       </c>
-      <c r="H38" s="5">
+      <c r="I38" s="5">
         <v>7800</v>
       </c>
-      <c r="I38" s="5">
+      <c r="J38" s="5">
         <v>3399.9999999999995</v>
       </c>
-      <c r="J38" s="6">
+      <c r="K38" s="6">
         <f t="shared" si="0"/>
         <v>4400</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A39" s="3">
         <v>306</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C39" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D39" s="1">
+      <c r="E39" s="1">
         <v>2022</v>
       </c>
-      <c r="E39" s="3">
+      <c r="F39" s="3">
         <v>306</v>
       </c>
-      <c r="F39" s="5">
+      <c r="G39" s="5">
         <v>4479.9999999999991</v>
       </c>
-      <c r="G39" s="5">
+      <c r="H39" s="5">
         <v>3540</v>
       </c>
-      <c r="H39" s="5">
+      <c r="I39" s="5">
         <v>8019.9999999999991</v>
       </c>
-      <c r="I39" s="5">
+      <c r="J39" s="5">
         <v>3540</v>
       </c>
-      <c r="J39" s="6">
+      <c r="K39" s="6">
         <f t="shared" si="0"/>
         <v>4479.9999999999991</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A40" s="3">
         <v>403</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C40" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D40" s="1">
+      <c r="E40" s="1">
         <v>2022</v>
       </c>
-      <c r="E40" s="3">
+      <c r="F40" s="3">
         <v>403</v>
       </c>
-      <c r="F40" s="5">
+      <c r="G40" s="5">
         <v>3600</v>
       </c>
-      <c r="G40" s="5">
+      <c r="H40" s="5">
         <v>3200</v>
       </c>
-      <c r="H40" s="5">
+      <c r="I40" s="5">
         <v>6800</v>
       </c>
-      <c r="I40" s="5">
+      <c r="J40" s="5">
         <v>3200</v>
       </c>
-      <c r="J40" s="6">
+      <c r="K40" s="6">
         <f t="shared" si="0"/>
         <v>3600</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A41" s="3">
         <v>501</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C41" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D41" s="1">
+      <c r="E41" s="1">
         <v>2022</v>
       </c>
-      <c r="E41" s="3">
+      <c r="F41" s="3">
         <v>501</v>
       </c>
-      <c r="F41" s="5">
+      <c r="G41" s="5">
         <v>5200</v>
       </c>
-      <c r="G41" s="5">
+      <c r="H41" s="5">
         <v>4300</v>
       </c>
-      <c r="H41" s="5">
+      <c r="I41" s="5">
         <v>9500</v>
       </c>
-      <c r="I41" s="5">
+      <c r="J41" s="5">
         <v>4300</v>
       </c>
-      <c r="J41" s="6">
+      <c r="K41" s="6">
         <f t="shared" si="0"/>
         <v>5200</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A42" s="2">
         <v>103</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C42" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D42" s="1">
+      <c r="E42" s="1">
         <v>2022</v>
       </c>
-      <c r="E42" s="2">
+      <c r="F42" s="2">
         <v>103</v>
       </c>
-      <c r="F42" s="5">
+      <c r="G42" s="5">
         <v>6404.24</v>
       </c>
-      <c r="G42" s="5">
+      <c r="H42" s="5">
         <v>10900</v>
       </c>
-      <c r="H42" s="5">
+      <c r="I42" s="5">
         <v>17304.239999999998</v>
       </c>
-      <c r="I42" s="5">
+      <c r="J42" s="5">
         <v>10900</v>
       </c>
-      <c r="J42" s="6">
+      <c r="K42" s="6">
         <f t="shared" si="0"/>
         <v>6404.239999999998</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A43" s="2">
         <v>204</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C43" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D43" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D43" s="1">
+      <c r="E43" s="1">
         <v>2022</v>
       </c>
-      <c r="E43" s="2">
+      <c r="F43" s="2">
         <v>204</v>
       </c>
-      <c r="F43" s="5">
+      <c r="G43" s="5">
         <v>9445.9999999999982</v>
       </c>
-      <c r="G43" s="5">
+      <c r="H43" s="5">
         <v>7000</v>
       </c>
-      <c r="H43" s="5">
+      <c r="I43" s="5">
         <v>16446</v>
       </c>
-      <c r="I43" s="5">
+      <c r="J43" s="5">
         <v>7000</v>
       </c>
-      <c r="J43" s="6">
+      <c r="K43" s="6">
         <f t="shared" si="0"/>
         <v>9446</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A44" s="2">
         <v>305</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C44" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D44" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D44" s="1">
+      <c r="E44" s="1">
         <v>2022</v>
       </c>
-      <c r="E44" s="2">
+      <c r="F44" s="2">
         <v>305</v>
       </c>
-      <c r="F44" s="5">
+      <c r="G44" s="5">
         <v>7103.9200000000028</v>
       </c>
-      <c r="G44" s="5">
+      <c r="H44" s="5">
         <v>8179.9999999999991</v>
       </c>
-      <c r="H44" s="5">
+      <c r="I44" s="5">
         <v>15283.920000000002</v>
       </c>
-      <c r="I44" s="5">
+      <c r="J44" s="5">
         <v>8179.9999999999991</v>
       </c>
-      <c r="J44" s="6">
+      <c r="K44" s="6">
         <f t="shared" si="0"/>
         <v>7103.9200000000028</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A45" s="2">
         <v>401</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C45" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D45" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D45" s="1">
+      <c r="E45" s="1">
         <v>2022</v>
       </c>
-      <c r="E45" s="2">
+      <c r="F45" s="2">
         <v>401</v>
       </c>
-      <c r="F45" s="5">
+      <c r="G45" s="5">
         <v>8927.1999999999989</v>
       </c>
-      <c r="G45" s="5">
+      <c r="H45" s="5">
         <v>8980</v>
       </c>
-      <c r="H45" s="5">
+      <c r="I45" s="5">
         <v>17907.199999999997</v>
       </c>
-      <c r="I45" s="5">
+      <c r="J45" s="5">
         <v>8980</v>
       </c>
-      <c r="J45" s="6">
+      <c r="K45" s="6">
         <f t="shared" si="0"/>
         <v>8927.1999999999971</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A46" s="2">
         <v>502</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C46" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D46" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D46" s="1">
+      <c r="E46" s="1">
         <v>2022</v>
       </c>
-      <c r="E46" s="2">
+      <c r="F46" s="2">
         <v>502</v>
       </c>
-      <c r="F46" s="5">
+      <c r="G46" s="5">
         <v>8457.2800000000007</v>
       </c>
-      <c r="G46" s="5">
+      <c r="H46" s="5">
         <v>11000</v>
       </c>
-      <c r="H46" s="5">
+      <c r="I46" s="5">
         <v>19457.28</v>
       </c>
-      <c r="I46" s="5">
+      <c r="J46" s="5">
         <v>11000</v>
       </c>
-      <c r="J46" s="6">
+      <c r="K46" s="6">
         <f t="shared" si="0"/>
         <v>8457.2799999999988</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A47" s="1">
         <v>105</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C47" s="2" t="s">
+      <c r="B47" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D47" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D47" s="1">
+      <c r="E47" s="1">
         <v>2022</v>
       </c>
-      <c r="E47" s="1">
+      <c r="F47" s="1">
         <v>105</v>
       </c>
-      <c r="F47" s="5">
+      <c r="G47" s="5">
         <v>7284.4</v>
       </c>
-      <c r="G47" s="5">
+      <c r="H47" s="5">
         <v>8560.0000000000018</v>
       </c>
-      <c r="H47" s="5">
+      <c r="I47" s="5">
         <v>15844.400000000001</v>
       </c>
-      <c r="I47" s="5">
+      <c r="J47" s="5">
         <v>8560.0000000000018</v>
       </c>
-      <c r="J47" s="6">
+      <c r="K47" s="6">
         <f t="shared" si="0"/>
         <v>7284.4</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A48" s="1">
         <v>203</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C48" s="2" t="s">
+      <c r="B48" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D48" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D48" s="1">
+      <c r="E48" s="1">
         <v>2022</v>
       </c>
-      <c r="E48" s="1">
+      <c r="F48" s="1">
         <v>203</v>
       </c>
-      <c r="F48" s="5">
+      <c r="G48" s="5">
         <v>7435.0400000000009</v>
       </c>
-      <c r="G48" s="5">
+      <c r="H48" s="5">
         <v>9360</v>
       </c>
-      <c r="H48" s="5">
+      <c r="I48" s="5">
         <v>16795.04</v>
       </c>
-      <c r="I48" s="5">
+      <c r="J48" s="5">
         <v>9360</v>
       </c>
-      <c r="J48" s="6">
+      <c r="K48" s="6">
         <f t="shared" si="0"/>
         <v>7435.0400000000009</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A49" s="1">
         <v>302</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C49" s="2" t="s">
+      <c r="B49" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D49" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D49" s="1">
+      <c r="E49" s="1">
         <v>2022</v>
       </c>
-      <c r="E49" s="1">
+      <c r="F49" s="1">
         <v>302</v>
       </c>
-      <c r="F49" s="5">
+      <c r="G49" s="5">
         <v>7555.92</v>
       </c>
-      <c r="G49" s="5">
+      <c r="H49" s="5">
         <v>8200</v>
       </c>
-      <c r="H49" s="5">
+      <c r="I49" s="5">
         <v>15755.92</v>
       </c>
-      <c r="I49" s="5">
+      <c r="J49" s="5">
         <v>8200</v>
       </c>
-      <c r="J49" s="6">
+      <c r="K49" s="6">
         <f t="shared" si="0"/>
         <v>7555.92</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A50" s="1">
         <v>406</v>
       </c>
-      <c r="B50" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C50" s="2" t="s">
+      <c r="B50" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D50" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D50" s="1">
+      <c r="E50" s="1">
         <v>2022</v>
       </c>
-      <c r="E50" s="1">
+      <c r="F50" s="1">
         <v>406</v>
       </c>
-      <c r="F50" s="5">
+      <c r="G50" s="5">
         <v>8633.52</v>
       </c>
-      <c r="G50" s="5">
+      <c r="H50" s="5">
         <v>8699.9999999999982</v>
       </c>
-      <c r="H50" s="5">
+      <c r="I50" s="5">
         <v>17333.519999999997</v>
       </c>
-      <c r="I50" s="5">
+      <c r="J50" s="5">
         <v>8699.9999999999982</v>
       </c>
-      <c r="J50" s="6">
+      <c r="K50" s="6">
         <f t="shared" si="0"/>
         <v>8633.5199999999986</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A51" s="1">
         <v>503</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C51" s="2" t="s">
+      <c r="B51" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D51" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D51" s="1">
+      <c r="E51" s="1">
         <v>2022</v>
       </c>
-      <c r="E51" s="1">
+      <c r="F51" s="1">
         <v>503</v>
       </c>
-      <c r="F51" s="5">
+      <c r="G51" s="5">
         <v>5118.9599999999991</v>
       </c>
-      <c r="G51" s="5">
+      <c r="H51" s="5">
         <v>6599.9999999999991</v>
       </c>
-      <c r="H51" s="5">
+      <c r="I51" s="5">
         <v>11718.96</v>
       </c>
-      <c r="I51" s="5">
+      <c r="J51" s="5">
         <v>6599.9999999999991</v>
       </c>
-      <c r="J51" s="6">
+      <c r="K51" s="6">
         <f t="shared" si="0"/>
         <v>5118.96</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A52" s="2">
         <v>101</v>
       </c>
-      <c r="B52" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C52" s="1" t="s">
+      <c r="B52" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D52" s="1">
+      <c r="E52" s="1">
         <v>2022</v>
       </c>
-      <c r="E52" s="2">
+      <c r="F52" s="2">
         <v>101</v>
       </c>
-      <c r="F52" s="5">
+      <c r="G52" s="5">
         <v>6580</v>
       </c>
-      <c r="G52" s="5"/>
-      <c r="H52" s="5">
-        <v>6580</v>
-      </c>
+      <c r="H52" s="5"/>
       <c r="I52" s="5">
         <v>6580</v>
       </c>
-      <c r="J52" s="6">
+      <c r="J52" s="5">
+        <v>6580</v>
+      </c>
+      <c r="K52" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A53" s="2">
         <v>205</v>
       </c>
-      <c r="B53" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C53" s="1" t="s">
+      <c r="B53" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D53" s="1">
+      <c r="E53" s="1">
         <v>2022</v>
       </c>
-      <c r="E53" s="2">
+      <c r="F53" s="2">
         <v>205</v>
       </c>
-      <c r="F53" s="5">
+      <c r="G53" s="5">
         <v>5560.0000000000009</v>
       </c>
-      <c r="G53" s="5"/>
-      <c r="H53" s="5">
-        <v>5560.0000000000009</v>
-      </c>
+      <c r="H53" s="5"/>
       <c r="I53" s="5">
         <v>5560.0000000000009</v>
       </c>
-      <c r="J53" s="6">
+      <c r="J53" s="5">
+        <v>5560.0000000000009</v>
+      </c>
+      <c r="K53" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A54" s="2">
         <v>303</v>
       </c>
-      <c r="B54" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C54" s="1" t="s">
+      <c r="B54" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D54" s="1">
+      <c r="E54" s="1">
         <v>2022</v>
       </c>
-      <c r="E54" s="2">
+      <c r="F54" s="2">
         <v>303</v>
       </c>
-      <c r="F54" s="5">
+      <c r="G54" s="5">
         <v>5740.0000000000009</v>
       </c>
-      <c r="G54" s="5"/>
-      <c r="H54" s="5">
-        <v>5740.0000000000009</v>
-      </c>
+      <c r="H54" s="5"/>
       <c r="I54" s="5">
         <v>5740.0000000000009</v>
       </c>
-      <c r="J54" s="6">
+      <c r="J54" s="5">
+        <v>5740.0000000000009</v>
+      </c>
+      <c r="K54" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A55" s="2">
         <v>404</v>
       </c>
-      <c r="B55" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C55" s="1" t="s">
+      <c r="B55" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D55" s="1">
+      <c r="E55" s="1">
         <v>2022</v>
       </c>
-      <c r="E55" s="2">
+      <c r="F55" s="2">
         <v>404</v>
       </c>
-      <c r="F55" s="5">
+      <c r="G55" s="5">
         <v>6880.0000000000009</v>
       </c>
-      <c r="G55" s="5"/>
-      <c r="H55" s="5">
-        <v>6880.0000000000009</v>
-      </c>
+      <c r="H55" s="5"/>
       <c r="I55" s="5">
         <v>6880.0000000000009</v>
       </c>
-      <c r="J55" s="6">
+      <c r="J55" s="5">
+        <v>6880.0000000000009</v>
+      </c>
+      <c r="K55" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A56" s="2">
         <v>506</v>
       </c>
-      <c r="B56" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C56" s="1" t="s">
+      <c r="B56" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D56" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D56" s="1">
+      <c r="E56" s="1">
         <v>2022</v>
       </c>
-      <c r="E56" s="2">
+      <c r="F56" s="2">
         <v>506</v>
       </c>
-      <c r="F56" s="5">
+      <c r="G56" s="5">
         <v>6480</v>
       </c>
-      <c r="G56" s="5"/>
-      <c r="H56" s="5">
-        <v>6480</v>
-      </c>
+      <c r="H56" s="5"/>
       <c r="I56" s="5">
         <v>6480</v>
       </c>
-      <c r="J56" s="6">
+      <c r="J56" s="5">
+        <v>6480</v>
+      </c>
+      <c r="K56" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A57" s="2">
         <v>102</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C57" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D57" s="1">
+      <c r="E57" s="1">
         <v>2022</v>
       </c>
-      <c r="E57" s="2">
+      <c r="F57" s="2">
         <v>102</v>
       </c>
-      <c r="F57" s="5">
+      <c r="G57" s="5">
         <v>3901.2000000000003</v>
       </c>
-      <c r="G57" s="5">
+      <c r="H57" s="5">
         <v>1138.8000000000002</v>
       </c>
-      <c r="H57" s="5">
+      <c r="I57" s="5">
         <v>5040</v>
       </c>
-      <c r="I57" s="5">
+      <c r="J57" s="5">
         <v>1138.8000000000002</v>
       </c>
-      <c r="J57" s="6">
+      <c r="K57" s="6">
         <f t="shared" si="0"/>
         <v>3901.2</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A58" s="2">
         <v>201</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C58" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D58" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D58" s="1">
+      <c r="E58" s="1">
         <v>2022</v>
       </c>
-      <c r="E58" s="2">
+      <c r="F58" s="2">
         <v>201</v>
       </c>
-      <c r="F58" s="5">
+      <c r="G58" s="5">
         <v>3955.2000000000003</v>
       </c>
-      <c r="G58" s="5">
+      <c r="H58" s="5">
         <v>1024.8</v>
       </c>
-      <c r="H58" s="5">
+      <c r="I58" s="5">
         <v>4980</v>
       </c>
-      <c r="I58" s="5">
+      <c r="J58" s="5">
         <v>1024.8</v>
       </c>
-      <c r="J58" s="6">
+      <c r="K58" s="6">
         <f t="shared" si="0"/>
         <v>3955.2</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A59" s="2">
         <v>304</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C59" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D59" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D59" s="1">
+      <c r="E59" s="1">
         <v>2022</v>
       </c>
-      <c r="E59" s="2">
+      <c r="F59" s="2">
         <v>304</v>
       </c>
-      <c r="F59" s="5">
+      <c r="G59" s="5">
         <v>4057.3999999999992</v>
       </c>
-      <c r="G59" s="5">
+      <c r="H59" s="5">
         <v>1242.5999999999999</v>
       </c>
-      <c r="H59" s="5">
+      <c r="I59" s="5">
         <v>5299.9999999999991</v>
       </c>
-      <c r="I59" s="5">
+      <c r="J59" s="5">
         <v>1242.5999999999999</v>
       </c>
-      <c r="J59" s="6">
+      <c r="K59" s="6">
         <f t="shared" si="0"/>
         <v>4057.3999999999992</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A60" s="2">
         <v>402</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C60" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D60" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D60" s="1">
+      <c r="E60" s="1">
         <v>2022</v>
       </c>
-      <c r="E60" s="2">
+      <c r="F60" s="2">
         <v>402</v>
       </c>
-      <c r="F60" s="5">
+      <c r="G60" s="5">
         <v>4459.2</v>
       </c>
-      <c r="G60" s="5">
+      <c r="H60" s="5">
         <v>1320.8</v>
       </c>
-      <c r="H60" s="5">
+      <c r="I60" s="5">
         <v>5780</v>
       </c>
-      <c r="I60" s="5">
+      <c r="J60" s="5">
         <v>1320.8</v>
       </c>
-      <c r="J60" s="6">
+      <c r="K60" s="6">
         <f t="shared" si="0"/>
         <v>4459.2</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A61" s="2">
         <v>505</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C61" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D61" s="1">
+      <c r="E61" s="1">
         <v>2022</v>
       </c>
-      <c r="E61" s="2">
+      <c r="F61" s="2">
         <v>505</v>
       </c>
-      <c r="F61" s="5">
+      <c r="G61" s="5">
         <v>5486.1999999999989</v>
       </c>
-      <c r="G61" s="5">
+      <c r="H61" s="5">
         <v>1533.8000000000002</v>
       </c>
-      <c r="H61" s="5">
+      <c r="I61" s="5">
         <v>7019.9999999999991</v>
       </c>
-      <c r="I61" s="5">
+      <c r="J61" s="5">
         <v>1533.8000000000002</v>
       </c>
-      <c r="J61" s="6">
+      <c r="K61" s="6">
         <f t="shared" si="0"/>
         <v>5486.1999999999989</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A62" s="2">
         <v>106</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C62" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D62" s="1">
+      <c r="E62" s="1">
         <v>2023</v>
       </c>
-      <c r="E62" s="2">
+      <c r="F62" s="2">
         <v>106</v>
       </c>
-      <c r="F62" s="5">
+      <c r="G62" s="5">
         <v>13873.240579710142</v>
       </c>
-      <c r="G62" s="5">
+      <c r="H62" s="5">
         <v>16219.999999999998</v>
       </c>
-      <c r="H62" s="5">
+      <c r="I62" s="5">
         <v>30093.240579710138</v>
       </c>
-      <c r="I62" s="5">
+      <c r="J62" s="5">
         <v>16219.999999999998</v>
       </c>
-      <c r="J62" s="6">
+      <c r="K62" s="6">
         <f t="shared" si="0"/>
         <v>13873.24057971014</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A63" s="2">
         <v>202</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C63" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D63" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D63" s="1">
+      <c r="E63" s="1">
         <v>2023</v>
       </c>
-      <c r="E63" s="2">
+      <c r="F63" s="2">
         <v>202</v>
       </c>
-      <c r="F63" s="5">
+      <c r="G63" s="5">
         <v>11726.332203389833</v>
       </c>
-      <c r="G63" s="5">
+      <c r="H63" s="5">
         <v>13619.999999999998</v>
       </c>
-      <c r="H63" s="5">
+      <c r="I63" s="5">
         <v>25346.332203389829</v>
       </c>
-      <c r="I63" s="5">
+      <c r="J63" s="5">
         <v>13619.999999999998</v>
       </c>
-      <c r="J63" s="6">
+      <c r="K63" s="6">
         <f t="shared" si="0"/>
         <v>11726.332203389831</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A64" s="2">
         <v>301</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C64" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D64" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D64" s="1">
+      <c r="E64" s="1">
         <v>2023</v>
       </c>
-      <c r="E64" s="2">
+      <c r="F64" s="2">
         <v>301</v>
       </c>
-      <c r="F64" s="5">
+      <c r="G64" s="5">
         <v>12413.665116279069</v>
       </c>
-      <c r="G64" s="5">
+      <c r="H64" s="5">
         <v>14360</v>
       </c>
-      <c r="H64" s="5">
+      <c r="I64" s="5">
         <v>26773.665116279069</v>
       </c>
-      <c r="I64" s="5">
+      <c r="J64" s="5">
         <v>14360</v>
       </c>
-      <c r="J64" s="6">
+      <c r="K64" s="6">
         <f t="shared" si="0"/>
         <v>12413.665116279069</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A65" s="2">
         <v>405</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C65" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D65" s="1">
+      <c r="E65" s="1">
         <v>2023</v>
       </c>
-      <c r="E65" s="2">
+      <c r="F65" s="2">
         <v>405</v>
       </c>
-      <c r="F65" s="5">
+      <c r="G65" s="5">
         <v>18779.127272727274</v>
       </c>
-      <c r="G65" s="5">
+      <c r="H65" s="5">
         <v>16720</v>
       </c>
-      <c r="H65" s="5">
+      <c r="I65" s="5">
         <v>35499.127272727274</v>
       </c>
-      <c r="I65" s="5">
+      <c r="J65" s="5">
         <v>16720</v>
       </c>
-      <c r="J65" s="6">
+      <c r="K65" s="6">
         <f t="shared" si="0"/>
         <v>18779.127272727274</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A66" s="2">
         <v>504</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C66" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D66" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D66" s="1">
+      <c r="E66" s="1">
         <v>2023</v>
       </c>
-      <c r="E66" s="2">
+      <c r="F66" s="2">
         <v>504</v>
       </c>
-      <c r="F66" s="5">
+      <c r="G66" s="5">
         <v>11745.637500000001</v>
       </c>
-      <c r="G66" s="5">
+      <c r="H66" s="5">
         <v>10960</v>
       </c>
-      <c r="H66" s="5">
+      <c r="I66" s="5">
         <v>22705.637500000001</v>
       </c>
-      <c r="I66" s="5">
+      <c r="J66" s="5">
         <v>10960</v>
       </c>
-      <c r="J66" s="6">
+      <c r="K66" s="6">
         <f t="shared" si="0"/>
         <v>11745.637500000001</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A67" s="3">
         <v>104</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C67" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D67" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D67" s="1">
+      <c r="E67" s="1">
         <v>2023</v>
       </c>
-      <c r="E67" s="3">
+      <c r="F67" s="3">
         <v>104</v>
       </c>
-      <c r="F67" s="5">
+      <c r="G67" s="5">
         <v>13980</v>
       </c>
-      <c r="G67" s="5"/>
-      <c r="H67" s="5">
-        <v>13980</v>
-      </c>
+      <c r="H67" s="5"/>
       <c r="I67" s="5">
         <v>13980</v>
       </c>
-      <c r="J67" s="6">
-        <f t="shared" ref="J67:J91" si="1">H67-I67</f>
+      <c r="J67" s="5">
+        <v>13980</v>
+      </c>
+      <c r="K67" s="6">
+        <f t="shared" ref="K67:K91" si="1">I67-J67</f>
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A68" s="3">
         <v>206</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C68" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D68" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D68" s="1">
+      <c r="E68" s="1">
         <v>2023</v>
       </c>
-      <c r="E68" s="3">
+      <c r="F68" s="3">
         <v>206</v>
       </c>
-      <c r="F68" s="5">
+      <c r="G68" s="5">
         <v>8480</v>
       </c>
-      <c r="G68" s="5"/>
-      <c r="H68" s="5">
-        <v>8480</v>
-      </c>
+      <c r="H68" s="5"/>
       <c r="I68" s="5">
         <v>8480</v>
       </c>
-      <c r="J68" s="6">
+      <c r="J68" s="5">
+        <v>8480</v>
+      </c>
+      <c r="K68" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A69" s="3">
         <v>306</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C69" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D69" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D69" s="1">
+      <c r="E69" s="1">
         <v>2023</v>
       </c>
-      <c r="E69" s="3">
+      <c r="F69" s="3">
         <v>306</v>
       </c>
-      <c r="F69" s="5">
+      <c r="G69" s="5">
         <v>10040</v>
       </c>
-      <c r="G69" s="5"/>
-      <c r="H69" s="5">
-        <v>10040</v>
-      </c>
+      <c r="H69" s="5"/>
       <c r="I69" s="5">
         <v>10040</v>
       </c>
-      <c r="J69" s="6">
+      <c r="J69" s="5">
+        <v>10040</v>
+      </c>
+      <c r="K69" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A70" s="3">
         <v>403</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C70" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D70" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D70" s="1">
+      <c r="E70" s="1">
         <v>2023</v>
       </c>
-      <c r="E70" s="3">
+      <c r="F70" s="3">
         <v>403</v>
       </c>
-      <c r="F70" s="5">
+      <c r="G70" s="5">
         <v>12120.000000000002</v>
       </c>
-      <c r="G70" s="5"/>
-      <c r="H70" s="5">
-        <v>12120.000000000002</v>
-      </c>
+      <c r="H70" s="5"/>
       <c r="I70" s="5">
         <v>12120.000000000002</v>
       </c>
-      <c r="J70" s="6">
+      <c r="J70" s="5">
+        <v>12120.000000000002</v>
+      </c>
+      <c r="K70" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A71" s="3">
         <v>501</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C71" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D71" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D71" s="1">
+      <c r="E71" s="1">
         <v>2023</v>
       </c>
-      <c r="E71" s="3">
+      <c r="F71" s="3">
         <v>501</v>
       </c>
-      <c r="F71" s="5">
+      <c r="G71" s="5">
         <v>11760.000000000002</v>
       </c>
-      <c r="G71" s="5"/>
-      <c r="H71" s="5">
-        <v>11760.000000000002</v>
-      </c>
+      <c r="H71" s="5"/>
       <c r="I71" s="5">
         <v>11760.000000000002</v>
       </c>
-      <c r="J71" s="6">
+      <c r="J71" s="5">
+        <v>11760.000000000002</v>
+      </c>
+      <c r="K71" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A72" s="2">
         <v>103</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C72" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D72" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D72" s="1">
+      <c r="E72" s="1">
         <v>2023</v>
       </c>
-      <c r="E72" s="2">
+      <c r="F72" s="2">
         <v>103</v>
       </c>
-      <c r="F72" s="5">
+      <c r="G72" s="5">
         <v>3620</v>
       </c>
-      <c r="G72" s="5">
+      <c r="H72" s="5">
         <v>4152</v>
       </c>
-      <c r="H72" s="5">
+      <c r="I72" s="5">
         <v>7772</v>
       </c>
-      <c r="I72" s="5">
+      <c r="J72" s="5">
         <v>4152</v>
       </c>
-      <c r="J72" s="6">
+      <c r="K72" s="6">
         <f t="shared" si="1"/>
         <v>3620</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A73" s="2">
         <v>204</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C73" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D73" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D73" s="1">
+      <c r="E73" s="1">
         <v>2023</v>
       </c>
-      <c r="E73" s="2">
+      <c r="F73" s="2">
         <v>204</v>
       </c>
-      <c r="F73" s="5">
+      <c r="G73" s="5">
         <v>3540</v>
       </c>
-      <c r="G73" s="5">
+      <c r="H73" s="5">
         <v>4056</v>
       </c>
-      <c r="H73" s="5">
+      <c r="I73" s="5">
         <v>7596</v>
       </c>
-      <c r="I73" s="5">
+      <c r="J73" s="5">
         <v>4056</v>
       </c>
-      <c r="J73" s="6">
+      <c r="K73" s="6">
         <f t="shared" si="1"/>
         <v>3540</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A74" s="2">
         <v>305</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C74" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D74" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D74" s="1">
+      <c r="E74" s="1">
         <v>2023</v>
       </c>
-      <c r="E74" s="2">
+      <c r="F74" s="2">
         <v>305</v>
       </c>
-      <c r="F74" s="5">
+      <c r="G74" s="5">
         <v>3620</v>
       </c>
-      <c r="G74" s="5">
+      <c r="H74" s="5">
         <v>4152</v>
       </c>
-      <c r="H74" s="5">
+      <c r="I74" s="5">
         <v>7772</v>
       </c>
-      <c r="I74" s="5">
+      <c r="J74" s="5">
         <v>4152</v>
       </c>
-      <c r="J74" s="6">
+      <c r="K74" s="6">
         <f t="shared" si="1"/>
         <v>3620</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A75" s="2">
         <v>401</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C75" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D75" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D75" s="1">
+      <c r="E75" s="1">
         <v>2023</v>
       </c>
-      <c r="E75" s="2">
+      <c r="F75" s="2">
         <v>401</v>
       </c>
-      <c r="F75" s="5">
+      <c r="G75" s="5">
         <v>4900.0000000000009</v>
       </c>
-      <c r="G75" s="5">
+      <c r="H75" s="5">
         <v>5400</v>
       </c>
-      <c r="H75" s="5">
+      <c r="I75" s="5">
         <v>10300</v>
       </c>
-      <c r="I75" s="5">
+      <c r="J75" s="5">
         <v>5400</v>
       </c>
-      <c r="J75" s="6">
+      <c r="K75" s="6">
         <f t="shared" si="1"/>
         <v>4900</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A76" s="2">
         <v>502</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C76" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D76" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D76" s="1">
+      <c r="E76" s="1">
         <v>2023</v>
       </c>
-      <c r="E76" s="2">
+      <c r="F76" s="2">
         <v>502</v>
       </c>
-      <c r="F76" s="5">
+      <c r="G76" s="5">
         <v>4480.0000000000009</v>
       </c>
-      <c r="G76" s="5">
+      <c r="H76" s="5">
         <v>5020</v>
       </c>
-      <c r="H76" s="5">
+      <c r="I76" s="5">
         <v>9500</v>
       </c>
-      <c r="I76" s="5">
+      <c r="J76" s="5">
         <v>5020</v>
       </c>
-      <c r="J76" s="6">
+      <c r="K76" s="6">
         <f t="shared" si="1"/>
         <v>4480</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A77" s="1">
         <v>105</v>
       </c>
-      <c r="B77" s="1" t="s">
-        <v>14</v>
+      <c r="B77" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C77" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D77" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D77" s="1">
+      <c r="E77" s="1">
         <v>2023</v>
       </c>
-      <c r="E77" s="1">
+      <c r="F77" s="1">
         <v>105</v>
       </c>
-      <c r="F77" s="5">
+      <c r="G77" s="5">
         <v>1990</v>
       </c>
-      <c r="G77" s="5">
+      <c r="H77" s="5">
         <v>670</v>
       </c>
-      <c r="H77" s="5">
+      <c r="I77" s="5">
         <v>2660</v>
       </c>
-      <c r="I77" s="5">
+      <c r="J77" s="5">
         <v>670</v>
       </c>
-      <c r="J77" s="6">
+      <c r="K77" s="6">
         <f t="shared" si="1"/>
         <v>1990</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A78" s="1">
         <v>203</v>
       </c>
-      <c r="B78" s="1" t="s">
-        <v>14</v>
+      <c r="B78" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C78" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D78" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D78" s="1">
+      <c r="E78" s="1">
         <v>2023</v>
       </c>
-      <c r="E78" s="1">
+      <c r="F78" s="1">
         <v>203</v>
       </c>
-      <c r="F78" s="5">
+      <c r="G78" s="5">
         <v>1810</v>
       </c>
-      <c r="G78" s="5">
+      <c r="H78" s="5">
         <v>630</v>
       </c>
-      <c r="H78" s="5">
+      <c r="I78" s="5">
         <v>2440</v>
       </c>
-      <c r="I78" s="5">
+      <c r="J78" s="5">
         <v>630</v>
       </c>
-      <c r="J78" s="6">
+      <c r="K78" s="6">
         <f t="shared" si="1"/>
         <v>1810</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A79" s="1">
         <v>302</v>
       </c>
-      <c r="B79" s="1" t="s">
-        <v>14</v>
+      <c r="B79" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C79" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D79" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D79" s="1">
+      <c r="E79" s="1">
         <v>2023</v>
       </c>
-      <c r="E79" s="1">
+      <c r="F79" s="1">
         <v>302</v>
       </c>
-      <c r="F79" s="5">
+      <c r="G79" s="5">
         <v>1692.0000000000002</v>
       </c>
-      <c r="G79" s="5">
+      <c r="H79" s="5">
         <v>448</v>
       </c>
-      <c r="H79" s="5">
+      <c r="I79" s="5">
         <v>2140</v>
       </c>
-      <c r="I79" s="5">
+      <c r="J79" s="5">
         <v>448</v>
       </c>
-      <c r="J79" s="6">
+      <c r="K79" s="6">
         <f t="shared" si="1"/>
         <v>1692</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A80" s="1">
         <v>406</v>
       </c>
-      <c r="B80" s="1" t="s">
-        <v>14</v>
+      <c r="B80" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C80" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D80" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D80" s="1">
+      <c r="E80" s="1">
         <v>2023</v>
       </c>
-      <c r="E80" s="1">
+      <c r="F80" s="1">
         <v>406</v>
       </c>
-      <c r="F80" s="5">
+      <c r="G80" s="5">
         <v>2304</v>
       </c>
-      <c r="G80" s="5">
+      <c r="H80" s="5">
         <v>356</v>
       </c>
-      <c r="H80" s="5">
+      <c r="I80" s="5">
         <v>2660</v>
       </c>
-      <c r="I80" s="5">
+      <c r="J80" s="5">
         <v>356</v>
       </c>
-      <c r="J80" s="6">
+      <c r="K80" s="6">
         <f t="shared" si="1"/>
         <v>2304</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A81" s="1">
         <v>503</v>
       </c>
-      <c r="B81" s="1" t="s">
-        <v>14</v>
+      <c r="B81" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C81" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D81" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D81" s="1">
+      <c r="E81" s="1">
         <v>2023</v>
       </c>
-      <c r="E81" s="1">
+      <c r="F81" s="1">
         <v>503</v>
       </c>
-      <c r="F81" s="5">
+      <c r="G81" s="5">
         <v>2226</v>
       </c>
-      <c r="G81" s="5">
+      <c r="H81" s="5">
         <v>354</v>
       </c>
-      <c r="H81" s="5">
+      <c r="I81" s="5">
         <v>2580</v>
       </c>
-      <c r="I81" s="5">
+      <c r="J81" s="5">
         <v>354</v>
       </c>
-      <c r="J81" s="6">
+      <c r="K81" s="6">
         <f t="shared" si="1"/>
         <v>2226</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A82" s="2">
         <v>101</v>
       </c>
-      <c r="B82" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C82" s="1" t="s">
+      <c r="B82" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D82" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D82" s="1">
+      <c r="E82" s="1">
         <v>2023</v>
       </c>
-      <c r="E82" s="2">
+      <c r="F82" s="2">
         <v>101</v>
       </c>
-      <c r="F82" s="5">
+      <c r="G82" s="5">
         <v>4360.0000000000009</v>
       </c>
-      <c r="G82" s="5">
+      <c r="H82" s="5">
         <v>4908</v>
       </c>
-      <c r="H82" s="5">
+      <c r="I82" s="5">
         <v>9268</v>
       </c>
-      <c r="I82" s="5">
+      <c r="J82" s="5">
         <v>4908</v>
       </c>
-      <c r="J82" s="6">
+      <c r="K82" s="6">
         <f t="shared" si="1"/>
         <v>4360</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A83" s="2">
         <v>205</v>
       </c>
-      <c r="B83" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C83" s="1" t="s">
+      <c r="B83" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D83" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D83" s="1">
+      <c r="E83" s="1">
         <v>2023</v>
       </c>
-      <c r="E83" s="2">
+      <c r="F83" s="2">
         <v>205</v>
       </c>
-      <c r="F83" s="5">
+      <c r="G83" s="5">
         <v>4059.9999999999995</v>
       </c>
-      <c r="G83" s="5">
+      <c r="H83" s="5">
         <v>4572</v>
       </c>
-      <c r="H83" s="5">
+      <c r="I83" s="5">
         <v>8632</v>
       </c>
-      <c r="I83" s="5">
+      <c r="J83" s="5">
         <v>4572</v>
       </c>
-      <c r="J83" s="6">
+      <c r="K83" s="6">
         <f t="shared" si="1"/>
         <v>4060</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A84" s="2">
         <v>303</v>
       </c>
-      <c r="B84" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C84" s="1" t="s">
+      <c r="B84" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D84" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D84" s="1">
+      <c r="E84" s="1">
         <v>2023</v>
       </c>
-      <c r="E84" s="2">
+      <c r="F84" s="2">
         <v>303</v>
       </c>
-      <c r="F84" s="5">
+      <c r="G84" s="5">
         <v>4080.0000000000009</v>
       </c>
-      <c r="G84" s="5">
+      <c r="H84" s="5">
         <v>4624</v>
       </c>
-      <c r="H84" s="5">
+      <c r="I84" s="5">
         <v>8704</v>
       </c>
-      <c r="I84" s="5">
+      <c r="J84" s="5">
         <v>4624</v>
       </c>
-      <c r="J84" s="6">
+      <c r="K84" s="6">
         <f t="shared" si="1"/>
         <v>4080</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A85" s="2">
         <v>404</v>
       </c>
-      <c r="B85" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C85" s="1" t="s">
+      <c r="B85" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D85" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D85" s="1">
+      <c r="E85" s="1">
         <v>2023</v>
       </c>
-      <c r="E85" s="2">
+      <c r="F85" s="2">
         <v>404</v>
       </c>
-      <c r="F85" s="5">
+      <c r="G85" s="5">
         <v>3960.0000000000009</v>
       </c>
-      <c r="G85" s="5">
+      <c r="H85" s="5">
         <v>4436</v>
       </c>
-      <c r="H85" s="5">
+      <c r="I85" s="5">
         <v>8396</v>
       </c>
-      <c r="I85" s="5">
+      <c r="J85" s="5">
         <v>4436</v>
       </c>
-      <c r="J85" s="6">
+      <c r="K85" s="6">
         <f t="shared" si="1"/>
         <v>3960</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A86" s="2">
         <v>506</v>
       </c>
-      <c r="B86" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C86" s="1" t="s">
+      <c r="B86" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D86" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D86" s="1">
+      <c r="E86" s="1">
         <v>2023</v>
       </c>
-      <c r="E86" s="2">
+      <c r="F86" s="2">
         <v>506</v>
       </c>
-      <c r="F86" s="5">
+      <c r="G86" s="5">
         <v>3319.9999999999995</v>
       </c>
-      <c r="G86" s="5">
+      <c r="H86" s="5">
         <v>3847.9999999999995</v>
       </c>
-      <c r="H86" s="5">
+      <c r="I86" s="5">
         <v>7167.9999999999991</v>
       </c>
-      <c r="I86" s="5">
+      <c r="J86" s="5">
         <v>3847.9999999999995</v>
       </c>
-      <c r="J86" s="6">
+      <c r="K86" s="6">
         <f t="shared" si="1"/>
         <v>3319.9999999999995</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A87" s="2">
         <v>102</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C87" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D87" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D87" s="1">
+      <c r="E87" s="1">
         <v>2023</v>
       </c>
-      <c r="E87" s="2">
+      <c r="F87" s="2">
         <v>102</v>
       </c>
-      <c r="F87" s="5">
+      <c r="G87" s="5">
         <v>14375.791304347827</v>
       </c>
-      <c r="G87" s="5">
+      <c r="H87" s="5">
         <v>15920</v>
       </c>
-      <c r="H87" s="5">
+      <c r="I87" s="5">
         <v>30295.791304347826</v>
       </c>
-      <c r="I87" s="5">
+      <c r="J87" s="5">
         <v>15920</v>
       </c>
-      <c r="J87" s="6">
+      <c r="K87" s="6">
         <f t="shared" si="1"/>
         <v>14375.791304347826</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A88" s="2">
         <v>201</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C88" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D88" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D88" s="1">
+      <c r="E88" s="1">
         <v>2023</v>
       </c>
-      <c r="E88" s="2">
+      <c r="F88" s="2">
         <v>201</v>
       </c>
-      <c r="F88" s="5">
+      <c r="G88" s="5">
         <v>10157.936448598135</v>
       </c>
-      <c r="G88" s="5">
+      <c r="H88" s="5">
         <v>15680</v>
       </c>
-      <c r="H88" s="5">
+      <c r="I88" s="5">
         <v>25837.936448598135</v>
       </c>
-      <c r="I88" s="5">
+      <c r="J88" s="5">
         <v>15680</v>
       </c>
-      <c r="J88" s="6">
+      <c r="K88" s="6">
         <f t="shared" si="1"/>
         <v>10157.936448598135</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A89" s="2">
         <v>304</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C89" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D89" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D89" s="1">
+      <c r="E89" s="1">
         <v>2023</v>
       </c>
-      <c r="E89" s="2">
+      <c r="F89" s="2">
         <v>304</v>
       </c>
-      <c r="F89" s="5">
+      <c r="G89" s="5">
         <v>10619.199999999999</v>
       </c>
-      <c r="G89" s="5">
+      <c r="H89" s="5">
         <v>11960.000000000002</v>
       </c>
-      <c r="H89" s="5">
+      <c r="I89" s="5">
         <v>22579.200000000001</v>
       </c>
-      <c r="I89" s="5">
+      <c r="J89" s="5">
         <v>11960.000000000002</v>
       </c>
-      <c r="J89" s="6">
+      <c r="K89" s="6">
         <f t="shared" si="1"/>
         <v>10619.199999999999</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A90" s="2">
         <v>402</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C90" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D90" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D90" s="1">
+      <c r="E90" s="1">
         <v>2023</v>
       </c>
-      <c r="E90" s="2">
+      <c r="F90" s="2">
         <v>402</v>
       </c>
-      <c r="F90" s="5">
+      <c r="G90" s="5">
         <v>13763.076923076924</v>
       </c>
-      <c r="G90" s="5">
+      <c r="H90" s="5">
         <v>15400</v>
       </c>
-      <c r="H90" s="5">
+      <c r="I90" s="5">
         <v>29163.076923076922</v>
       </c>
-      <c r="I90" s="5">
+      <c r="J90" s="5">
         <v>15400</v>
       </c>
-      <c r="J90" s="6">
+      <c r="K90" s="6">
         <f t="shared" si="1"/>
         <v>13763.076923076922</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A91" s="2">
         <v>505</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C91" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D91" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D91" s="1">
+      <c r="E91" s="1">
         <v>2023</v>
       </c>
-      <c r="E91" s="2">
+      <c r="F91" s="2">
         <v>505</v>
       </c>
-      <c r="F91" s="5">
+      <c r="G91" s="5">
         <v>12687.341176470594</v>
       </c>
-      <c r="G91" s="5">
+      <c r="H91" s="5">
         <v>14720</v>
       </c>
-      <c r="H91" s="5">
+      <c r="I91" s="5">
         <v>27407.341176470596</v>
       </c>
-      <c r="I91" s="5">
+      <c r="J91" s="5">
         <v>14720</v>
       </c>
-      <c r="J91" s="6">
+      <c r="K91" s="6">
         <f t="shared" si="1"/>
         <v>12687.341176470596</v>
       </c>

</xml_diff>